<commit_message>
Adicionado arquivo de Backlog e modificiado arquivo de Requisitos
</commit_message>
<xml_diff>
--- a/docs/Requisitos_pi.xlsx
+++ b/docs/Requisitos_pi.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28103"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="292" documentId="11_7F4755BF84DCCE43E268565A8931F45BFA75341E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B83173EB-4DE7-4B68-AE6A-309197089275}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="11_7F4755BF84DCCE43E268565A8931F45BFA75341E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D930C2-48AD-4ED9-AD1B-97F6D5D10A2E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Requisitos da Aplicação</t>
   </si>
@@ -105,7 +105,7 @@
     <t>Criação da Tabela manutenção</t>
   </si>
   <si>
-    <t>Criação da tabela manutenação, que irá registrar as manutenções realizadas</t>
+    <t>Criação da tabela manutenção, que irá registrar as manutenções realizadas</t>
   </si>
   <si>
     <t>Site Institucional</t>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Barra superior para que o usário consiga navegar facilmente entre as sessões do site.</t>
+  </si>
+  <si>
+    <t>Criação da Tabela empresa</t>
+  </si>
+  <si>
+    <t>Criação da tabela empresa, que irá registrar as empresas clientes</t>
   </si>
   <si>
     <t>Área de dashboard</t>
@@ -354,6 +360,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,14 +399,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -851,7 +867,7 @@
   <dimension ref="A1:AE14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:G7"/>
+      <selection activeCell="Y4" sqref="Y4:AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,130 +880,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="9" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="9" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="6"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="7"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="4"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="8"/>
     </row>
     <row r="3" spans="1:31" ht="84.75" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="15" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="15" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15" t="s">
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15" t="s">
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="7"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="8"/>
     </row>
     <row r="4" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1003,7 +1019,7 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="5"/>
       <c r="L4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1035,7 @@
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
-      <c r="U4" s="4"/>
+      <c r="U4" s="5"/>
       <c r="V4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1035,10 +1051,10 @@
       </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="7"/>
+      <c r="AE4" s="8"/>
     </row>
     <row r="5" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1054,7 +1070,7 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="5"/>
       <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1070,7 +1086,7 @@
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="4"/>
+      <c r="U5" s="5"/>
       <c r="V5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1086,10 +1102,10 @@
       </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="7"/>
+      <c r="AE5" s="8"/>
     </row>
     <row r="6" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1121,7 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1121,7 +1137,7 @@
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="4"/>
+      <c r="U6" s="5"/>
       <c r="V6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1137,10 +1153,10 @@
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="7"/>
+      <c r="AE6" s="8"/>
     </row>
     <row r="7" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1156,7 +1172,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1172,20 +1188,26 @@
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="2"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="Y7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
+      <c r="AB7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="7"/>
+      <c r="AE7" s="8"/>
     </row>
     <row r="8" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1195,14 +1217,14 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="4"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1211,7 +1233,7 @@
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="U8" s="4"/>
+      <c r="U8" s="5"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
@@ -1221,10 +1243,10 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="7"/>
+      <c r="AE8" s="8"/>
     </row>
     <row r="9" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1234,14 +1256,14 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="4"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1250,7 +1272,7 @@
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
-      <c r="U9" s="4"/>
+      <c r="U9" s="5"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
@@ -1260,10 +1282,10 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="7"/>
+      <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1273,23 +1295,23 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="4"/>
+      <c r="K10" s="5"/>
       <c r="L10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="U10" s="4"/>
+      <c r="U10" s="5"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
@@ -1299,10 +1321,10 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="7"/>
+      <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1312,23 +1334,23 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="4"/>
+      <c r="K11" s="5"/>
       <c r="L11" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="4"/>
+      <c r="U11" s="5"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
@@ -1338,10 +1360,10 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="7"/>
+      <c r="AE11" s="8"/>
     </row>
     <row r="12" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1351,23 +1373,23 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="4"/>
+      <c r="K12" s="5"/>
       <c r="L12" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-      <c r="U12" s="4"/>
+      <c r="U12" s="5"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
@@ -1377,10 +1399,10 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="7"/>
+      <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1390,23 +1412,23 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="4"/>
+      <c r="U13" s="5"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
@@ -1416,10 +1438,10 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
-      <c r="AE13" s="7"/>
+      <c r="AE13" s="8"/>
     </row>
     <row r="14" spans="1:31" ht="80.25" customHeight="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1429,23 +1451,23 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-      <c r="U14" s="5"/>
+      <c r="U14" s="6"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
@@ -1453,34 +1475,85 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
-      <c r="AE14" s="8"/>
+      <c r="AE14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="Y8:AA8"/>
-    <mergeCell ref="AB8:AD8"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AB12:AD12"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="A1:A14"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="U1:U14"/>
+    <mergeCell ref="AE1:AE14"/>
+    <mergeCell ref="V1:AD2"/>
+    <mergeCell ref="L1:T2"/>
+    <mergeCell ref="K1:K14"/>
+    <mergeCell ref="B1:J2"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R8:T8"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="AB3:AD3"/>
@@ -1505,134 +1578,88 @@
     <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="AB14:AD14"/>
     <mergeCell ref="V11:X11"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="U1:U14"/>
-    <mergeCell ref="AE1:AE14"/>
-    <mergeCell ref="V1:AD2"/>
-    <mergeCell ref="L1:T2"/>
-    <mergeCell ref="K1:K14"/>
-    <mergeCell ref="B1:J2"/>
-    <mergeCell ref="A1:A14"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="AB8:AD8"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="AB12:AD12"/>
   </mergeCells>
   <conditionalFormatting sqref="R3:T14">
+    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:J3">
     <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:J3">
+  <conditionalFormatting sqref="J18">
     <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
-      <formula>"Essencial"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="9" priority="23" operator="equal">
       <formula>"Importante$AD$4"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD14">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="23" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD6 R4:T14">
-    <cfRule type="cellIs" dxfId="7" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD14">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB4:AD14 R4:T14">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+  <conditionalFormatting sqref="R4:T14 AB4:AD14">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J14">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J14">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J14">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB7:AD7 AB9:AD14">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB8:AD8">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB8:AD8">
+  <conditionalFormatting sqref="AB7:AD7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>

</xml_diff>